<commit_message>
bunch of primary analysis
</commit_message>
<xml_diff>
--- a/Delay Test Exp 3.xlsx
+++ b/Delay Test Exp 3.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/d201901_hiroshima-u_ac_jp/Documents/Doctoral Course 2020/Experiments/OOP_Maya/last experiment files/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/d201901_hiroshima-u_ac_jp/Documents/Doctoral Course 2020/Experiments/OOP_Maya/last experiment files/OOP-experiment-data-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_BE3751A7D5A5422755F96970B502D8EBC1EB9EBA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EBCE05D-BA69-4EA3-BBC7-EC3D6C8156DF}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_BE3751A7D5A5422755F96970B502D8EBC1EB9EBA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FC1D2FC-3819-427D-B418-523D0C68D3F0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1155" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25365" yWindow="585" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBO.21.22.1 (Presensi 7AB) Reme" sheetId="1" r:id="rId1"/>
     <sheet name="RAW" sheetId="2" r:id="rId2"/>
-    <sheet name="delay score" sheetId="3" r:id="rId3"/>
+    <sheet name="timeinsecond" sheetId="4" r:id="rId3"/>
+    <sheet name="delay score" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'delay score'!$B$2</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'delay score'!$B$3:$B$44</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'delay score'!$B$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'delay score'!$B$3:$B$44</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'delay score'!$E$1:$F$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'delay score'!$F$3:$F$38</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'delay score'!$E$1:$F$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'delay score'!$F$3:$F$38</definedName>
     <definedName name="delay_score">RAW!$H$1:$H$109</definedName>
     <definedName name="stid">RAW!$B$1:$B$109</definedName>
   </definedNames>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3987" uniqueCount="542">
   <si>
     <t>Nama akhir</t>
   </si>
@@ -1676,6 +1675,24 @@
   </si>
   <si>
     <t>1402018163</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>total_second</t>
   </si>
 </sst>
 </file>
@@ -1718,10 +1735,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1755,12 +1772,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1771,7 +1788,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000001-D6B2-4B3C-88A8-6C279DFC9A48}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>delay_score</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1783,7 +1800,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000002-D6B2-4B3C-88A8-6C279DFC9A48}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v/>
             </cx:txData>
           </cx:tx>
@@ -10571,8 +10588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB110"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20028,14 +20045,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705FB666-35A5-4F83-A6FD-ED1691FFB021}">
   <dimension ref="A1:AB110"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.125" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -29486,11 +29503,2645 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370CBC97-538C-4F12-B3CA-493302846105}">
+  <dimension ref="A1:H109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1" t="s">
+        <v>538</v>
+      </c>
+      <c r="F1" t="s">
+        <v>539</v>
+      </c>
+      <c r="G1" t="s">
+        <v>540</v>
+      </c>
+      <c r="H1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1402020069</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>95</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>24</v>
+      </c>
+      <c r="H2">
+        <f>(F2*60)+G2</f>
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1402020066</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H66" si="0">(F3*60)+G3</f>
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1402020035</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1402019043</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <f>(F5*60)+G5</f>
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1402020117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="F6">
+        <v>28</v>
+      </c>
+      <c r="G6">
+        <v>36</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1402020029</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1402017084</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1402019099</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1402020031</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1402020079</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>36</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>936</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1402017148</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1402020072</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1402020041</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1402020016</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1402017036</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>782</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1402020083</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17">
+        <v>85</v>
+      </c>
+      <c r="F17">
+        <v>29</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1402020027</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18">
+        <v>90</v>
+      </c>
+      <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1402017065</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19">
+        <v>45</v>
+      </c>
+      <c r="F19">
+        <v>25</v>
+      </c>
+      <c r="G19">
+        <v>54</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1402018185</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20">
+        <v>65</v>
+      </c>
+      <c r="F20">
+        <v>29</v>
+      </c>
+      <c r="G20">
+        <v>49</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1402020043</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21">
+        <v>75</v>
+      </c>
+      <c r="F21">
+        <v>28</v>
+      </c>
+      <c r="G21">
+        <v>59</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1402020057</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22">
+        <v>85</v>
+      </c>
+      <c r="F22">
+        <v>22</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1402019036</v>
+      </c>
+      <c r="B23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23">
+        <v>70</v>
+      </c>
+      <c r="F23">
+        <v>29</v>
+      </c>
+      <c r="G23">
+        <v>59</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1402019048</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24">
+        <v>45</v>
+      </c>
+      <c r="F24">
+        <v>27</v>
+      </c>
+      <c r="G24">
+        <v>55</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1402020034</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25">
+        <v>60</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>37</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1402017066</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26">
+        <v>65</v>
+      </c>
+      <c r="F26">
+        <v>27</v>
+      </c>
+      <c r="G26">
+        <v>20</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1402020101</v>
+      </c>
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27">
+        <v>30</v>
+      </c>
+      <c r="F27">
+        <v>27</v>
+      </c>
+      <c r="G27">
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1402020033</v>
+      </c>
+      <c r="B28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28">
+        <v>75</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1402020090</v>
+      </c>
+      <c r="B29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29">
+        <v>65</v>
+      </c>
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1402020064</v>
+      </c>
+      <c r="B30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30">
+        <v>35</v>
+      </c>
+      <c r="F30">
+        <v>29</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1402020070</v>
+      </c>
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31">
+        <v>70</v>
+      </c>
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31">
+        <v>46</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1402020059</v>
+      </c>
+      <c r="B32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32">
+        <v>80</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1402019040</v>
+      </c>
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" t="s">
+        <v>181</v>
+      </c>
+      <c r="D33">
+        <v>50</v>
+      </c>
+      <c r="F33">
+        <v>17</v>
+      </c>
+      <c r="G33">
+        <v>22</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1402017049</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>28</v>
+      </c>
+      <c r="G34">
+        <v>15</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1402020133</v>
+      </c>
+      <c r="B35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35">
+        <v>60</v>
+      </c>
+      <c r="F35">
+        <v>28</v>
+      </c>
+      <c r="G35">
+        <v>39</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1402020102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" t="s">
+        <v>193</v>
+      </c>
+      <c r="D36">
+        <v>45</v>
+      </c>
+      <c r="F36">
+        <v>29</v>
+      </c>
+      <c r="G36">
+        <v>16</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1402020114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>197</v>
+      </c>
+      <c r="C37" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37">
+        <v>80</v>
+      </c>
+      <c r="F37">
+        <v>29</v>
+      </c>
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1402020039</v>
+      </c>
+      <c r="B38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38">
+        <v>85</v>
+      </c>
+      <c r="F38">
+        <v>30</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1402020076</v>
+      </c>
+      <c r="B39" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" t="s">
+        <v>206</v>
+      </c>
+      <c r="D39">
+        <v>90</v>
+      </c>
+      <c r="F39">
+        <v>29</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1402020023</v>
+      </c>
+      <c r="B40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C40" t="s">
+        <v>210</v>
+      </c>
+      <c r="D40">
+        <v>35</v>
+      </c>
+      <c r="F40">
+        <v>28</v>
+      </c>
+      <c r="G40">
+        <v>42</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1402018119</v>
+      </c>
+      <c r="B41" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" t="s">
+        <v>215</v>
+      </c>
+      <c r="D41">
+        <v>30</v>
+      </c>
+      <c r="F41">
+        <v>21</v>
+      </c>
+      <c r="G41">
+        <v>22</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1402019045</v>
+      </c>
+      <c r="B42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C42" t="s">
+        <v>219</v>
+      </c>
+      <c r="D42">
+        <v>75</v>
+      </c>
+      <c r="F42">
+        <v>29</v>
+      </c>
+      <c r="G42">
+        <v>56</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1402020116</v>
+      </c>
+      <c r="B43" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" t="s">
+        <v>223</v>
+      </c>
+      <c r="D43">
+        <v>85</v>
+      </c>
+      <c r="F43">
+        <v>28</v>
+      </c>
+      <c r="G43">
+        <v>17</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1402020080</v>
+      </c>
+      <c r="B44" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" t="s">
+        <v>227</v>
+      </c>
+      <c r="D44">
+        <v>90</v>
+      </c>
+      <c r="F44">
+        <v>22</v>
+      </c>
+      <c r="G44">
+        <v>20</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1402020052</v>
+      </c>
+      <c r="B45" t="s">
+        <v>197</v>
+      </c>
+      <c r="C45" t="s">
+        <v>231</v>
+      </c>
+      <c r="D45">
+        <v>60</v>
+      </c>
+      <c r="F45">
+        <v>27</v>
+      </c>
+      <c r="G45">
+        <v>10</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1402020008</v>
+      </c>
+      <c r="B46" t="s">
+        <v>197</v>
+      </c>
+      <c r="C46" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46">
+        <v>90</v>
+      </c>
+      <c r="F46">
+        <v>29</v>
+      </c>
+      <c r="G46">
+        <v>59</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1402020067</v>
+      </c>
+      <c r="B47" t="s">
+        <v>238</v>
+      </c>
+      <c r="C47" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47">
+        <v>50</v>
+      </c>
+      <c r="F47">
+        <v>29</v>
+      </c>
+      <c r="G47">
+        <v>31</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1402016052</v>
+      </c>
+      <c r="B48" t="s">
+        <v>238</v>
+      </c>
+      <c r="C48" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48">
+        <v>45</v>
+      </c>
+      <c r="F48">
+        <v>20</v>
+      </c>
+      <c r="G48">
+        <v>32</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1402020135</v>
+      </c>
+      <c r="B49" t="s">
+        <v>238</v>
+      </c>
+      <c r="C49" t="s">
+        <v>247</v>
+      </c>
+      <c r="D49">
+        <v>55</v>
+      </c>
+      <c r="F49">
+        <v>29</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1402020112</v>
+      </c>
+      <c r="B50" t="s">
+        <v>238</v>
+      </c>
+      <c r="C50" t="s">
+        <v>252</v>
+      </c>
+      <c r="D50">
+        <v>85</v>
+      </c>
+      <c r="F50">
+        <v>25</v>
+      </c>
+      <c r="G50">
+        <v>49</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1402020081</v>
+      </c>
+      <c r="B51" t="s">
+        <v>238</v>
+      </c>
+      <c r="C51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51">
+        <v>90</v>
+      </c>
+      <c r="F51">
+        <v>30</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1402020007</v>
+      </c>
+      <c r="B52" t="s">
+        <v>238</v>
+      </c>
+      <c r="C52" t="s">
+        <v>260</v>
+      </c>
+      <c r="D52">
+        <v>35</v>
+      </c>
+      <c r="F52">
+        <v>27</v>
+      </c>
+      <c r="G52">
+        <v>8</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1402020103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>238</v>
+      </c>
+      <c r="C53" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53">
+        <v>85</v>
+      </c>
+      <c r="F53">
+        <v>24</v>
+      </c>
+      <c r="G53">
+        <v>6</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1402018187</v>
+      </c>
+      <c r="B54" t="s">
+        <v>238</v>
+      </c>
+      <c r="C54" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54">
+        <v>55</v>
+      </c>
+      <c r="F54">
+        <v>30</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1402020087</v>
+      </c>
+      <c r="B55" t="s">
+        <v>238</v>
+      </c>
+      <c r="C55" t="s">
+        <v>271</v>
+      </c>
+      <c r="D55">
+        <v>80</v>
+      </c>
+      <c r="F55">
+        <v>29</v>
+      </c>
+      <c r="G55">
+        <v>9</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="0"/>
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1402018229</v>
+      </c>
+      <c r="B56" t="s">
+        <v>238</v>
+      </c>
+      <c r="C56" t="s">
+        <v>275</v>
+      </c>
+      <c r="D56">
+        <v>35</v>
+      </c>
+      <c r="F56">
+        <v>29</v>
+      </c>
+      <c r="G56">
+        <v>44</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="0"/>
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1402020063</v>
+      </c>
+      <c r="B57" t="s">
+        <v>238</v>
+      </c>
+      <c r="C57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57">
+        <v>90</v>
+      </c>
+      <c r="F57">
+        <v>30</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="0"/>
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1402020137</v>
+      </c>
+      <c r="B58" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D58">
+        <v>45</v>
+      </c>
+      <c r="F58">
+        <v>29</v>
+      </c>
+      <c r="G58">
+        <v>34</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="0"/>
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1402020019</v>
+      </c>
+      <c r="B59" t="s">
+        <v>238</v>
+      </c>
+      <c r="C59" t="s">
+        <v>286</v>
+      </c>
+      <c r="D59">
+        <v>80</v>
+      </c>
+      <c r="F59">
+        <v>27</v>
+      </c>
+      <c r="G59">
+        <v>34</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="0"/>
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1402020098</v>
+      </c>
+      <c r="B60" t="s">
+        <v>290</v>
+      </c>
+      <c r="C60" t="s">
+        <v>291</v>
+      </c>
+      <c r="D60">
+        <v>70</v>
+      </c>
+      <c r="F60">
+        <v>23</v>
+      </c>
+      <c r="G60">
+        <v>48</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="0"/>
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1402020053</v>
+      </c>
+      <c r="B61" t="s">
+        <v>290</v>
+      </c>
+      <c r="C61" t="s">
+        <v>296</v>
+      </c>
+      <c r="D61">
+        <v>45</v>
+      </c>
+      <c r="F61">
+        <v>30</v>
+      </c>
+      <c r="G61">
+        <v>26</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="0"/>
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1402020107</v>
+      </c>
+      <c r="B62" t="s">
+        <v>290</v>
+      </c>
+      <c r="C62" t="s">
+        <v>300</v>
+      </c>
+      <c r="D62">
+        <v>85</v>
+      </c>
+      <c r="F62">
+        <v>29</v>
+      </c>
+      <c r="G62">
+        <v>53</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="0"/>
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1402020074</v>
+      </c>
+      <c r="B63" t="s">
+        <v>290</v>
+      </c>
+      <c r="C63" t="s">
+        <v>304</v>
+      </c>
+      <c r="D63">
+        <v>60</v>
+      </c>
+      <c r="F63">
+        <v>28</v>
+      </c>
+      <c r="G63">
+        <v>50</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="0"/>
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1402020062</v>
+      </c>
+      <c r="B64" t="s">
+        <v>290</v>
+      </c>
+      <c r="C64" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64">
+        <v>90</v>
+      </c>
+      <c r="F64">
+        <v>30</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1402020065</v>
+      </c>
+      <c r="B65" t="s">
+        <v>290</v>
+      </c>
+      <c r="C65" t="s">
+        <v>311</v>
+      </c>
+      <c r="D65">
+        <v>85</v>
+      </c>
+      <c r="F65">
+        <v>28</v>
+      </c>
+      <c r="G65">
+        <v>22</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="0"/>
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1402020095</v>
+      </c>
+      <c r="B66" t="s">
+        <v>290</v>
+      </c>
+      <c r="C66" t="s">
+        <v>315</v>
+      </c>
+      <c r="D66">
+        <v>75</v>
+      </c>
+      <c r="F66">
+        <v>24</v>
+      </c>
+      <c r="G66">
+        <v>40</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="0"/>
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1402017019</v>
+      </c>
+      <c r="B67" t="s">
+        <v>290</v>
+      </c>
+      <c r="C67" t="s">
+        <v>319</v>
+      </c>
+      <c r="D67">
+        <v>30</v>
+      </c>
+      <c r="F67">
+        <v>19</v>
+      </c>
+      <c r="G67">
+        <v>34</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H110" si="1">(F67*60)+G67</f>
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1402020097</v>
+      </c>
+      <c r="B68" t="s">
+        <v>290</v>
+      </c>
+      <c r="C68" t="s">
+        <v>324</v>
+      </c>
+      <c r="D68">
+        <v>100</v>
+      </c>
+      <c r="F68">
+        <v>16</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="1"/>
+        <v>961</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1402020134</v>
+      </c>
+      <c r="B69" t="s">
+        <v>329</v>
+      </c>
+      <c r="C69" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69">
+        <v>80</v>
+      </c>
+      <c r="F69">
+        <v>30</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="1"/>
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1402020032</v>
+      </c>
+      <c r="B70" t="s">
+        <v>329</v>
+      </c>
+      <c r="C70" t="s">
+        <v>334</v>
+      </c>
+      <c r="D70">
+        <v>80</v>
+      </c>
+      <c r="F70">
+        <v>29</v>
+      </c>
+      <c r="G70">
+        <v>21</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="1"/>
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1402020030</v>
+      </c>
+      <c r="B71" t="s">
+        <v>329</v>
+      </c>
+      <c r="C71" t="s">
+        <v>338</v>
+      </c>
+      <c r="D71">
+        <v>95</v>
+      </c>
+      <c r="F71">
+        <v>26</v>
+      </c>
+      <c r="G71">
+        <v>55</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="1"/>
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1402019074</v>
+      </c>
+      <c r="B72" t="s">
+        <v>342</v>
+      </c>
+      <c r="C72" t="s">
+        <v>343</v>
+      </c>
+      <c r="D72">
+        <v>80</v>
+      </c>
+      <c r="F72">
+        <v>27</v>
+      </c>
+      <c r="G72">
+        <v>28</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="1"/>
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1402020054</v>
+      </c>
+      <c r="B73" t="s">
+        <v>342</v>
+      </c>
+      <c r="C73" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73">
+        <v>55</v>
+      </c>
+      <c r="F73">
+        <v>24</v>
+      </c>
+      <c r="G73">
+        <v>37</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="1"/>
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1402020073</v>
+      </c>
+      <c r="B74" t="s">
+        <v>342</v>
+      </c>
+      <c r="C74" t="s">
+        <v>247</v>
+      </c>
+      <c r="D74">
+        <v>55</v>
+      </c>
+      <c r="F74">
+        <v>29</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="1"/>
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1402020005</v>
+      </c>
+      <c r="B75" t="s">
+        <v>342</v>
+      </c>
+      <c r="C75" t="s">
+        <v>353</v>
+      </c>
+      <c r="D75">
+        <v>75</v>
+      </c>
+      <c r="F75">
+        <v>28</v>
+      </c>
+      <c r="G75">
+        <v>41</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="1"/>
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1402020061</v>
+      </c>
+      <c r="B76" t="s">
+        <v>342</v>
+      </c>
+      <c r="C76" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76">
+        <v>75</v>
+      </c>
+      <c r="F76">
+        <v>30</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1402020058</v>
+      </c>
+      <c r="B77" t="s">
+        <v>342</v>
+      </c>
+      <c r="C77" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77">
+        <v>55</v>
+      </c>
+      <c r="F77">
+        <v>30</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1402020021</v>
+      </c>
+      <c r="B78" t="s">
+        <v>342</v>
+      </c>
+      <c r="C78" t="s">
+        <v>77</v>
+      </c>
+      <c r="D78">
+        <v>60</v>
+      </c>
+      <c r="F78">
+        <v>30</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1402020115</v>
+      </c>
+      <c r="B79" t="s">
+        <v>342</v>
+      </c>
+      <c r="C79" t="s">
+        <v>168</v>
+      </c>
+      <c r="D79">
+        <v>70</v>
+      </c>
+      <c r="F79">
+        <v>29</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="1"/>
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1402020025</v>
+      </c>
+      <c r="B80" t="s">
+        <v>370</v>
+      </c>
+      <c r="C80" t="s">
+        <v>123</v>
+      </c>
+      <c r="D80">
+        <v>50</v>
+      </c>
+      <c r="F80">
+        <v>29</v>
+      </c>
+      <c r="G80">
+        <v>49</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="1"/>
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1402019086</v>
+      </c>
+      <c r="B81" t="s">
+        <v>370</v>
+      </c>
+      <c r="C81" t="s">
+        <v>374</v>
+      </c>
+      <c r="D81">
+        <v>70</v>
+      </c>
+      <c r="F81">
+        <v>21</v>
+      </c>
+      <c r="G81">
+        <v>9</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="1"/>
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1402019028</v>
+      </c>
+      <c r="B82" t="s">
+        <v>370</v>
+      </c>
+      <c r="C82" t="s">
+        <v>379</v>
+      </c>
+      <c r="D82">
+        <v>60</v>
+      </c>
+      <c r="F82">
+        <v>29</v>
+      </c>
+      <c r="G82">
+        <v>54</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="1"/>
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1402018076</v>
+      </c>
+      <c r="B83" t="s">
+        <v>370</v>
+      </c>
+      <c r="C83" t="s">
+        <v>138</v>
+      </c>
+      <c r="D83">
+        <v>60</v>
+      </c>
+      <c r="F83">
+        <v>29</v>
+      </c>
+      <c r="G83">
+        <v>59</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="1"/>
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1402020113</v>
+      </c>
+      <c r="B84" t="s">
+        <v>370</v>
+      </c>
+      <c r="C84" t="s">
+        <v>386</v>
+      </c>
+      <c r="D84">
+        <v>85</v>
+      </c>
+      <c r="F84">
+        <v>27</v>
+      </c>
+      <c r="G84">
+        <v>43</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="1"/>
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1402019046</v>
+      </c>
+      <c r="B85" t="s">
+        <v>370</v>
+      </c>
+      <c r="C85" t="s">
+        <v>77</v>
+      </c>
+      <c r="D85">
+        <v>80</v>
+      </c>
+      <c r="F85">
+        <v>30</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1402020128</v>
+      </c>
+      <c r="B86" t="s">
+        <v>370</v>
+      </c>
+      <c r="C86" t="s">
+        <v>393</v>
+      </c>
+      <c r="D86">
+        <v>30</v>
+      </c>
+      <c r="F86">
+        <v>28</v>
+      </c>
+      <c r="G86">
+        <v>33</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="1"/>
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1402020089</v>
+      </c>
+      <c r="B87" t="s">
+        <v>397</v>
+      </c>
+      <c r="C87" t="s">
+        <v>398</v>
+      </c>
+      <c r="D87">
+        <v>95</v>
+      </c>
+      <c r="F87">
+        <v>19</v>
+      </c>
+      <c r="G87">
+        <v>42</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="1"/>
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1402020124</v>
+      </c>
+      <c r="B88" t="s">
+        <v>397</v>
+      </c>
+      <c r="C88" t="s">
+        <v>109</v>
+      </c>
+      <c r="D88">
+        <v>60</v>
+      </c>
+      <c r="F88">
+        <v>29</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="1"/>
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1402019005</v>
+      </c>
+      <c r="B89" t="s">
+        <v>397</v>
+      </c>
+      <c r="C89" t="s">
+        <v>405</v>
+      </c>
+      <c r="D89">
+        <v>65</v>
+      </c>
+      <c r="F89">
+        <v>29</v>
+      </c>
+      <c r="G89">
+        <v>23</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="1"/>
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1402020088</v>
+      </c>
+      <c r="B90" t="s">
+        <v>397</v>
+      </c>
+      <c r="C90" t="s">
+        <v>409</v>
+      </c>
+      <c r="D90">
+        <v>70</v>
+      </c>
+      <c r="F90">
+        <v>23</v>
+      </c>
+      <c r="G90">
+        <v>11</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="1"/>
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1402019038</v>
+      </c>
+      <c r="B91" t="s">
+        <v>397</v>
+      </c>
+      <c r="C91" t="s">
+        <v>77</v>
+      </c>
+      <c r="D91">
+        <v>60</v>
+      </c>
+      <c r="F91">
+        <v>30</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1402019071</v>
+      </c>
+      <c r="B92" t="s">
+        <v>397</v>
+      </c>
+      <c r="C92" t="s">
+        <v>417</v>
+      </c>
+      <c r="D92">
+        <v>85</v>
+      </c>
+      <c r="F92">
+        <v>26</v>
+      </c>
+      <c r="G92">
+        <v>2</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="1"/>
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1402019069</v>
+      </c>
+      <c r="B93" t="s">
+        <v>397</v>
+      </c>
+      <c r="C93" t="s">
+        <v>421</v>
+      </c>
+      <c r="D93">
+        <v>80</v>
+      </c>
+      <c r="F93">
+        <v>22</v>
+      </c>
+      <c r="G93">
+        <v>54</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="1"/>
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1402019024</v>
+      </c>
+      <c r="B94" t="s">
+        <v>397</v>
+      </c>
+      <c r="C94" t="s">
+        <v>95</v>
+      </c>
+      <c r="D94">
+        <v>80</v>
+      </c>
+      <c r="F94">
+        <v>30</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="1"/>
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1402019009</v>
+      </c>
+      <c r="B95" t="s">
+        <v>428</v>
+      </c>
+      <c r="C95" t="s">
+        <v>429</v>
+      </c>
+      <c r="D95">
+        <v>85</v>
+      </c>
+      <c r="F95">
+        <v>18</v>
+      </c>
+      <c r="G95">
+        <v>39</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="1"/>
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1402020132</v>
+      </c>
+      <c r="B96" t="s">
+        <v>428</v>
+      </c>
+      <c r="C96" t="s">
+        <v>231</v>
+      </c>
+      <c r="D96">
+        <v>65</v>
+      </c>
+      <c r="F96">
+        <v>27</v>
+      </c>
+      <c r="G96">
+        <v>10</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="1"/>
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1402020111</v>
+      </c>
+      <c r="B97" t="s">
+        <v>428</v>
+      </c>
+      <c r="C97" t="s">
+        <v>315</v>
+      </c>
+      <c r="D97">
+        <v>80</v>
+      </c>
+      <c r="F97">
+        <v>24</v>
+      </c>
+      <c r="G97">
+        <v>40</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="1"/>
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1402019001</v>
+      </c>
+      <c r="B98" t="s">
+        <v>439</v>
+      </c>
+      <c r="C98" t="s">
+        <v>440</v>
+      </c>
+      <c r="D98">
+        <v>40</v>
+      </c>
+      <c r="F98">
+        <v>27</v>
+      </c>
+      <c r="G98">
+        <v>39</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="1"/>
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>1402020075</v>
+      </c>
+      <c r="B99" t="s">
+        <v>439</v>
+      </c>
+      <c r="C99" t="s">
+        <v>445</v>
+      </c>
+      <c r="D99">
+        <v>90</v>
+      </c>
+      <c r="F99">
+        <v>21</v>
+      </c>
+      <c r="G99">
+        <v>35</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="1"/>
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1402018198</v>
+      </c>
+      <c r="B100" t="s">
+        <v>449</v>
+      </c>
+      <c r="C100" t="s">
+        <v>450</v>
+      </c>
+      <c r="D100">
+        <v>60</v>
+      </c>
+      <c r="F100">
+        <v>23</v>
+      </c>
+      <c r="G100">
+        <v>21</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="1"/>
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>1402019008</v>
+      </c>
+      <c r="B101" t="s">
+        <v>449</v>
+      </c>
+      <c r="C101" t="s">
+        <v>454</v>
+      </c>
+      <c r="D101">
+        <v>45</v>
+      </c>
+      <c r="F101">
+        <v>22</v>
+      </c>
+      <c r="G101">
+        <v>6</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="1"/>
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1402020086</v>
+      </c>
+      <c r="B102" t="s">
+        <v>449</v>
+      </c>
+      <c r="C102" t="s">
+        <v>458</v>
+      </c>
+      <c r="D102">
+        <v>65</v>
+      </c>
+      <c r="F102">
+        <v>26</v>
+      </c>
+      <c r="G102">
+        <v>56</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="1"/>
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1402020138</v>
+      </c>
+      <c r="B103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C103" t="s">
+        <v>462</v>
+      </c>
+      <c r="D103">
+        <v>60</v>
+      </c>
+      <c r="F103">
+        <v>18</v>
+      </c>
+      <c r="G103">
+        <v>17</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="1"/>
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1402018221</v>
+      </c>
+      <c r="B104" t="s">
+        <v>466</v>
+      </c>
+      <c r="C104" t="s">
+        <v>467</v>
+      </c>
+      <c r="D104">
+        <v>50</v>
+      </c>
+      <c r="F104">
+        <v>25</v>
+      </c>
+      <c r="G104">
+        <v>16</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="1"/>
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1402019077</v>
+      </c>
+      <c r="B105" t="s">
+        <v>82</v>
+      </c>
+      <c r="C105" t="s">
+        <v>471</v>
+      </c>
+      <c r="D105">
+        <v>30</v>
+      </c>
+      <c r="F105">
+        <v>16</v>
+      </c>
+      <c r="G105">
+        <v>14</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="1"/>
+        <v>974</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1402020092</v>
+      </c>
+      <c r="B106" t="s">
+        <v>475</v>
+      </c>
+      <c r="C106" t="s">
+        <v>476</v>
+      </c>
+      <c r="D106">
+        <v>65</v>
+      </c>
+      <c r="F106">
+        <v>21</v>
+      </c>
+      <c r="G106">
+        <v>48</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="1"/>
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1402019021</v>
+      </c>
+      <c r="B107" t="s">
+        <v>480</v>
+      </c>
+      <c r="C107" t="s">
+        <v>481</v>
+      </c>
+      <c r="D107">
+        <v>65</v>
+      </c>
+      <c r="F107">
+        <v>17</v>
+      </c>
+      <c r="G107">
+        <v>31</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="1"/>
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>1402019098</v>
+      </c>
+      <c r="B108" t="s">
+        <v>180</v>
+      </c>
+      <c r="C108" t="s">
+        <v>485</v>
+      </c>
+      <c r="D108">
+        <v>90</v>
+      </c>
+      <c r="F108">
+        <v>11</v>
+      </c>
+      <c r="G108">
+        <v>22</v>
+      </c>
+      <c r="H108">
+        <f t="shared" si="1"/>
+        <v>682</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1402020056</v>
+      </c>
+      <c r="B109" t="s">
+        <v>323</v>
+      </c>
+      <c r="C109" t="s">
+        <v>489</v>
+      </c>
+      <c r="D109">
+        <v>35</v>
+      </c>
+      <c r="F109">
+        <v>6</v>
+      </c>
+      <c r="G109">
+        <v>4</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="1"/>
+        <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AF4328-7BAA-4BFC-B75E-3273BD7E490A}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -29501,14 +32152,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -29541,7 +32192,7 @@
         <f>VLOOKUP(E3,RAW!$B$2:$H$109,7,FALSE)</f>
         <v>85</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>362</v>
       </c>
     </row>
@@ -29560,7 +32211,7 @@
         <f>VLOOKUP(E4,RAW!$B$2:$H$109,7,FALSE)</f>
         <v>90</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>443</v>
       </c>
     </row>
@@ -29579,7 +32230,7 @@
         <f>VLOOKUP(E5,RAW!$B$2:$H$109,7,FALSE)</f>
         <v>80</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -29598,7 +32249,7 @@
         <f>VLOOKUP(E6,RAW!$B$2:$H$109,7,FALSE)</f>
         <v>65</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>175</v>
       </c>
     </row>
@@ -29617,7 +32268,7 @@
         <f>VLOOKUP(E7,RAW!$B$2:$H$109,7,FALSE)</f>
         <v>85</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -29636,7 +32287,7 @@
         <f>VLOOKUP(E8,RAW!$B$2:$H$109,7,FALSE)</f>
         <v>90</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>535</v>
       </c>
     </row>

</xml_diff>